<commit_message>
Update json and csv files (v4).
</commit_message>
<xml_diff>
--- a/JSON/Levels4.xlsx
+++ b/JSON/Levels4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emchar1/Documents/Xcode Projects/Projects/PUZL Boy/JSON/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3909F9-E27B-7C4D-A8F2-02E37F6F92A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2381C3F-3EBF-E54A-870C-7026491D2E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3394" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="87">
   <si>
     <t>health</t>
   </si>
@@ -439,7 +439,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,18 +661,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -834,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -844,8 +832,6 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1201,13 +1187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BX139"/>
+  <dimension ref="A1:BX140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1508,7 @@
         <f>A2+1</f>
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="6">
         <f t="shared" ref="B3:B66" si="0">A3</f>
         <v>1</v>
       </c>
@@ -1848,7 +1834,7 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -2113,7 +2099,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="6">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -2368,7 +2354,7 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -2543,7 +2529,7 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -3003,7 +2989,7 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="6">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -3474,7 +3460,7 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="6">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
@@ -15995,7 +15981,7 @@
     </row>
     <row r="132" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A132" s="6">
-        <f t="shared" ref="A132:A139" si="5">A131+1</f>
+        <f t="shared" ref="A132:A140" si="5">A131+1</f>
         <v>130</v>
       </c>
       <c r="B132" s="6">
@@ -17136,6 +17122,160 @@
       <c r="BW139" s="8"/>
       <c r="BX139" s="8"/>
     </row>
+    <row r="140" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="A140" s="6">
+        <f t="shared" si="5"/>
+        <v>138</v>
+      </c>
+      <c r="B140" s="6">
+        <f t="shared" ref="B140" si="6">A140</f>
+        <v>138</v>
+      </c>
+      <c r="C140">
+        <v>23</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>75</v>
+      </c>
+      <c r="F140" t="s">
+        <v>85</v>
+      </c>
+      <c r="G140" t="s">
+        <v>81</v>
+      </c>
+      <c r="H140" t="s">
+        <v>81</v>
+      </c>
+      <c r="I140" t="s">
+        <v>81</v>
+      </c>
+      <c r="K140" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="L140" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="M140" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="N140" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O140" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="P140" s="7"/>
+      <c r="Q140" t="s">
+        <v>81</v>
+      </c>
+      <c r="R140" t="s">
+        <v>85</v>
+      </c>
+      <c r="S140" t="s">
+        <v>81</v>
+      </c>
+      <c r="T140" t="s">
+        <v>85</v>
+      </c>
+      <c r="U140" t="s">
+        <v>81</v>
+      </c>
+      <c r="W140" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="X140" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y140" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z140" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA140" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB140" s="7"/>
+      <c r="AC140" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD140" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE140" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF140" t="s">
+        <v>85</v>
+      </c>
+      <c r="AG140" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI140" s="7"/>
+      <c r="AJ140" s="7"/>
+      <c r="AK140" s="7"/>
+      <c r="AL140" s="7"/>
+      <c r="AM140" s="7"/>
+      <c r="AN140" s="7"/>
+      <c r="AP140" t="s">
+        <v>79</v>
+      </c>
+      <c r="AQ140" t="s">
+        <v>78</v>
+      </c>
+      <c r="AU140" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="AV140" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW140" s="8"/>
+      <c r="AX140" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AY140" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="AZ140" s="8"/>
+      <c r="BA140" t="s">
+        <v>78</v>
+      </c>
+      <c r="BB140" t="s">
+        <v>79</v>
+      </c>
+      <c r="BC140" t="s">
+        <v>78</v>
+      </c>
+      <c r="BD140" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG140" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="BH140" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BI140" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ140" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="BK140" s="8"/>
+      <c r="BL140" s="8"/>
+      <c r="BP140" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS140" s="8"/>
+      <c r="BT140" s="8"/>
+      <c r="BU140" s="8"/>
+      <c r="BV140" s="8"/>
+      <c r="BW140" s="8"/>
+      <c r="BX140" s="8"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:BX139" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>